<commit_message>
Excel Sheet - Corrected Initial onhand, Need to work on final time period
</commit_message>
<xml_diff>
--- a/src/dynamiclot/excel/Algo_Test.xlsx
+++ b/src/dynamiclot/excel/Algo_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dynamicLot\dynamicLot\src\dynamiclot\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F7DD88-519A-42ED-848D-525AF14A52AE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1663D2D5-AF3D-4644-80E5-172D86EB0C9A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{02BB62FB-2EF9-455F-95E9-05B9DFC2DF15}"/>
   </bookViews>
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1A9ADD-C05D-4DA2-985E-8370FA174CA3}">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView topLeftCell="D6" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,15 +816,15 @@
         <v>31</v>
       </c>
       <c r="M9" s="2">
-        <f>K9-L9</f>
+        <f t="shared" ref="M9:M23" si="0">K9-L9</f>
         <v>31</v>
       </c>
       <c r="N9" s="2">
-        <f>IF(M9 &gt;= 0,0,1)</f>
+        <f t="shared" ref="N9:N14" si="1">IF(M9 &gt;= 0,0,1)</f>
         <v>0</v>
       </c>
       <c r="O9" s="3">
-        <f>IF(N9=1,IF(ABS(M9)&lt;=IF(SUMPRODUCT(C9:D9,G9:H9)&lt;=0,MIN(G9:H9),SUMPRODUCT(C9:D9,G9:H9)),ABS(M9),IF(SUMPRODUCT(C9:D9,G9:H9)&lt;=0,MIN(G9:H9),SUMPRODUCT(C9:D9,G9:H9))),0)</f>
+        <f t="shared" ref="O9:O23" si="2">IF(N9=1,IF(ABS(M9)&lt;=IF(SUMPRODUCT(C9:D9,G9:H9)&lt;=0,MIN(G9:H9),SUMPRODUCT(C9:D9,G9:H9)),ABS(M9),IF(SUMPRODUCT(C9:D9,G9:H9)&lt;=0,MIN(G9:H9),SUMPRODUCT(C9:D9,G9:H9))),0)</f>
         <v>0</v>
       </c>
       <c r="P9" s="3">
@@ -832,15 +832,15 @@
         <v>1</v>
       </c>
       <c r="Q9">
-        <f t="shared" ref="Q9:Q11" si="0">IF(R9&gt;0, IF(O9&gt;=0,O9,0),0)</f>
+        <f t="shared" ref="Q9:Q11" si="3">IF(R9&gt;0, IF(O9&gt;=0,O9,0),0)</f>
         <v>0</v>
       </c>
       <c r="R9">
-        <f t="shared" ref="R9:R20" si="1">IF(SUMPRODUCT(C9:D9,G9:H9)&gt;0,1,0)</f>
+        <f t="shared" ref="R9:R20" si="4">IF(SUMPRODUCT(C9:D9,G9:H9)&gt;0,1,0)</f>
         <v>0</v>
       </c>
       <c r="S9">
-        <f t="shared" ref="S9:S20" si="2">Q9-O9</f>
+        <f t="shared" ref="S9:S20" si="5">Q9-O9</f>
         <v>0</v>
       </c>
     </row>
@@ -858,11 +858,11 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <f t="shared" ref="G10:H23" si="3">$B$1</f>
+        <f t="shared" ref="G10:H23" si="6">$B$1</f>
         <v>118</v>
       </c>
       <c r="H10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="I10">
@@ -881,15 +881,15 @@
         <v>31</v>
       </c>
       <c r="M10">
-        <f>K10-L10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N10">
-        <f>IF(M10 &gt;= 0,0,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O10" s="5">
-        <f>IF(N10=1,IF(ABS(M10)&lt;=IF(SUMPRODUCT(C10:D10,G10:H10)&lt;=0,MIN(G10:H10),SUMPRODUCT(C10:D10,G10:H10)),ABS(M10),IF(SUMPRODUCT(C10:D10,G10:H10)&lt;=0,MIN(G10:H10),SUMPRODUCT(C10:D10,G10:H10))),0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P10" s="5">
@@ -897,15 +897,15 @@
         <v>1</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -925,11 +925,11 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="H11" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="I11" s="7">
@@ -948,28 +948,28 @@
         <v>31</v>
       </c>
       <c r="M11" s="7">
-        <f>K11-L11</f>
+        <f t="shared" si="0"/>
         <v>-31</v>
       </c>
       <c r="N11" s="7">
-        <f>IF(M11 &gt;= 0,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O11" s="8">
-        <f>IF(N11=1,IF(ABS(M11)&lt;=IF(SUMPRODUCT(C11:D11,G11:H11)&lt;=0,MIN(G11:H11),SUMPRODUCT(C11:D11,G11:H11)),ABS(M11),IF(SUMPRODUCT(C11:D11,G11:H11)&lt;=0,MIN(G11:H11),SUMPRODUCT(C11:D11,G11:H11))),0)</f>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="P11" s="5"/>
       <c r="Q11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="R11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="S11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1012,28 +1012,28 @@
         <v>60</v>
       </c>
       <c r="M12" s="2">
-        <f>K12-L12</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="N12" s="2">
-        <f>IF(M12 &gt;= 0,0,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O12" s="3">
-        <f>IF(N12=1,IF(ABS(M12)&lt;=IF(SUMPRODUCT(C12:D12,G12:H12)&lt;=0,MIN(G12:H12),SUMPRODUCT(C12:D12,G12:H12)),ABS(M12),IF(SUMPRODUCT(C12:D12,G12:H12)&lt;=0,MIN(G12:H12),SUMPRODUCT(C12:D12,G12:H12))),0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P12" s="5"/>
       <c r="Q12">
-        <f t="shared" ref="Q12:Q14" si="4">IF(R12&gt;0, IF(O12&gt;=0,O12,0),0)</f>
+        <f t="shared" ref="Q12:Q14" si="7">IF(R12&gt;0, IF(O12&gt;=0,O12,0),0)</f>
         <v>0</v>
       </c>
       <c r="R12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1051,11 +1051,11 @@
         <v>1</v>
       </c>
       <c r="G13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="H13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="I13">
@@ -1074,28 +1074,28 @@
         <v>60</v>
       </c>
       <c r="M13">
-        <f>K13-L13</f>
+        <f t="shared" si="0"/>
         <v>-50</v>
       </c>
       <c r="N13">
-        <f>IF(M13 &gt;= 0,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O13" s="5">
-        <f>IF(N13=1,IF(ABS(M13)&lt;=IF(SUMPRODUCT(C13:D13,G13:H13)&lt;=0,MIN(G13:H13),SUMPRODUCT(C13:D13,G13:H13)),ABS(M13),IF(SUMPRODUCT(C13:D13,G13:H13)&lt;=0,MIN(G13:H13),SUMPRODUCT(C13:D13,G13:H13))),0)</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="P13" s="5"/>
       <c r="Q13">
+        <f t="shared" si="7"/>
+        <v>50</v>
+      </c>
+      <c r="R13">
         <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="R13">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="S13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1115,11 +1115,11 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="H14" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="I14" s="7">
@@ -1138,28 +1138,28 @@
         <v>60</v>
       </c>
       <c r="M14" s="7">
-        <f>K14-L14</f>
+        <f t="shared" si="0"/>
         <v>-60</v>
       </c>
       <c r="N14" s="7">
-        <f>IF(M14 &gt;= 0,0,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O14" s="8">
-        <f>IF(N14=1,IF(ABS(M14)&lt;=IF(SUMPRODUCT(C14:D14,G14:H14)&lt;=0,MIN(G14:H14),SUMPRODUCT(C14:D14,G14:H14)),ABS(M14),IF(SUMPRODUCT(C14:D14,G14:H14)&lt;=0,MIN(G14:H14),SUMPRODUCT(C14:D14,G14:H14))),0)</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="P14" s="5"/>
       <c r="Q14">
+        <f t="shared" si="7"/>
+        <v>60</v>
+      </c>
+      <c r="R14">
         <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-      <c r="R14">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="S14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1202,15 +1202,15 @@
         <v>17</v>
       </c>
       <c r="M15" s="2">
-        <f>K15-L15</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="N15" s="2">
-        <f t="shared" ref="N15" si="5">IF(M15 &gt;= 0,0,1)</f>
+        <f t="shared" ref="N15" si="8">IF(M15 &gt;= 0,0,1)</f>
         <v>0</v>
       </c>
       <c r="O15" s="3">
-        <f>IF(N15=1,IF(ABS(M15)&lt;=IF(SUMPRODUCT(C15:D15,G15:H15)&lt;=0,MIN(G15:H15),SUMPRODUCT(C15:D15,G15:H15)),ABS(M15),IF(SUMPRODUCT(C15:D15,G15:H15)&lt;=0,MIN(G15:H15),SUMPRODUCT(C15:D15,G15:H15))),0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P15" s="5">
@@ -1218,15 +1218,15 @@
         <v>1</v>
       </c>
       <c r="Q15">
-        <f t="shared" ref="Q15:Q17" si="6">IF(R15&gt;0, IF(O15&gt;=0,O15,0),0)</f>
+        <f t="shared" ref="Q15:Q17" si="9">IF(R15&gt;0, IF(O15&gt;=0,O15,0),0)</f>
         <v>0</v>
       </c>
       <c r="R15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1244,11 +1244,11 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="H16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="I16">
@@ -1267,15 +1267,15 @@
         <v>17</v>
       </c>
       <c r="M16">
-        <f>K16-L16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N16">
-        <f>IF(M16 &gt;= 0,0,1)</f>
+        <f t="shared" ref="N16:N23" si="10">IF(M16 &gt;= 0,0,1)</f>
         <v>0</v>
       </c>
       <c r="O16" s="5">
-        <f>IF(N16=1,IF(ABS(M16)&lt;=IF(SUMPRODUCT(C16:D16,G16:H16)&lt;=0,MIN(G16:H16),SUMPRODUCT(C16:D16,G16:H16)),ABS(M16),IF(SUMPRODUCT(C16:D16,G16:H16)&lt;=0,MIN(G16:H16),SUMPRODUCT(C16:D16,G16:H16))),0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P16" s="5">
@@ -1283,15 +1283,15 @@
         <v>1</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1311,11 +1311,11 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="H17" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="I17" s="7">
@@ -1334,15 +1334,15 @@
         <v>17</v>
       </c>
       <c r="M17" s="7">
-        <f>K17-L17</f>
+        <f t="shared" si="0"/>
         <v>-17</v>
       </c>
       <c r="N17" s="7">
-        <f>IF(M17 &gt;= 0,0,1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="O17" s="8">
-        <f>IF(N17=1,IF(ABS(M17)&lt;=IF(SUMPRODUCT(C17:D17,G17:H17)&lt;=0,MIN(G17:H17),SUMPRODUCT(C17:D17,G17:H17)),ABS(M17),IF(SUMPRODUCT(C17:D17,G17:H17)&lt;=0,MIN(G17:H17),SUMPRODUCT(C17:D17,G17:H17))),0)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="P17" s="5">
@@ -1350,15 +1350,15 @@
         <v>1</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="R17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="S17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1378,11 +1378,11 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="I18" s="2">
@@ -1401,28 +1401,28 @@
         <v>38</v>
       </c>
       <c r="M18" s="2">
-        <f>K18-L18</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="N18" s="2">
-        <f>IF(M18 &gt;= 0,0,1)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O18" s="3">
-        <f>IF(N18=1,IF(ABS(M18)&lt;=IF(SUMPRODUCT(C18:D18,G18:H18)&lt;=0,MIN(G18:H18),SUMPRODUCT(C18:D18,G18:H18)),ABS(M18),IF(SUMPRODUCT(C18:D18,G18:H18)&lt;=0,MIN(G18:H18),SUMPRODUCT(C18:D18,G18:H18))),0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P18" s="5"/>
       <c r="Q18">
-        <f t="shared" ref="Q18:Q20" si="7">IF(R18&gt;0, IF(O18&gt;=0,O18,0),0)</f>
+        <f t="shared" ref="Q18:Q20" si="11">IF(R18&gt;0, IF(O18&gt;=0,O18,0),0)</f>
         <v>0</v>
       </c>
       <c r="R18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1440,11 +1440,11 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="H19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="I19">
@@ -1463,15 +1463,15 @@
         <v>38</v>
       </c>
       <c r="M19">
-        <f>K19-L19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N19">
-        <f>IF(M19 &gt;= 0,0,1)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O19" s="5">
-        <f>IF(N19=1,IF(ABS(M19)&lt;=IF(SUMPRODUCT(C19:D19,G19:H19)&lt;=0,MIN(G19:H19),SUMPRODUCT(C19:D19,G19:H19)),ABS(M19),IF(SUMPRODUCT(C19:D19,G19:H19)&lt;=0,MIN(G19:H19),SUMPRODUCT(C19:D19,G19:H19))),0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P19" s="5">
@@ -1479,15 +1479,15 @@
         <v>1</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1507,11 +1507,11 @@
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="H20" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="I20" s="7">
@@ -1530,27 +1530,27 @@
         <v>38</v>
       </c>
       <c r="M20" s="7">
-        <f>K20-L20</f>
+        <f t="shared" si="0"/>
         <v>-38</v>
       </c>
       <c r="N20" s="7">
-        <f>IF(M20 &gt;= 0,0,1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="O20" s="8">
-        <f>IF(N20=1,IF(ABS(M20)&lt;=IF(SUMPRODUCT(C20:D20,G20:H20)&lt;=0,MIN(G20:H20),SUMPRODUCT(C20:D20,G20:H20)),ABS(M20),IF(SUMPRODUCT(C20:D20,G20:H20)&lt;=0,MIN(G20:H20),SUMPRODUCT(C20:D20,G20:H20))),0)</f>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>38</v>
       </c>
       <c r="R20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="S20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1570,11 +1570,11 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="I21" s="2">
@@ -1593,15 +1593,15 @@
         <v>12</v>
       </c>
       <c r="M21" s="2">
-        <f>K21-L21</f>
+        <f t="shared" si="0"/>
         <v>-2</v>
       </c>
       <c r="N21" s="2">
-        <f>IF(M21 &gt;= 0,0,1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="O21" s="3">
-        <f>IF(N21=1,IF(ABS(M21)&lt;=IF(SUMPRODUCT(C21:D21,G21:H21)&lt;=0,MIN(G21:H21),SUMPRODUCT(C21:D21,G21:H21)),ABS(M21),IF(SUMPRODUCT(C21:D21,G21:H21)&lt;=0,MIN(G21:H21),SUMPRODUCT(C21:D21,G21:H21))),0)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Q21">
@@ -1631,11 +1631,11 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="H22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="I22">
@@ -1654,15 +1654,15 @@
         <v>12</v>
       </c>
       <c r="M22">
-        <f>K22-L22</f>
+        <f t="shared" si="0"/>
         <v>-12</v>
       </c>
       <c r="N22">
-        <f>IF(M22 &gt;= 0,0,1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="O22" s="5">
-        <f>IF(N22=1,IF(ABS(M22)&lt;=IF(SUMPRODUCT(C22:D22,G22:H22)&lt;=0,MIN(G22:H22),SUMPRODUCT(C22:D22,G22:H22)),ABS(M22),IF(SUMPRODUCT(C22:D22,G22:H22)&lt;=0,MIN(G22:H22),SUMPRODUCT(C22:D22,G22:H22))),0)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="Q22">
@@ -1694,11 +1694,11 @@
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="H23" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118</v>
       </c>
       <c r="I23" s="7">
@@ -1717,15 +1717,15 @@
         <v>12</v>
       </c>
       <c r="M23" s="7">
-        <f>K23-L23</f>
+        <f t="shared" si="0"/>
         <v>-12</v>
       </c>
       <c r="N23" s="7">
-        <f>IF(M23 &gt;= 0,0,1)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="O23" s="8">
-        <f>IF(N23=1,IF(ABS(M23)&lt;=IF(SUMPRODUCT(C23:D23,G23:H23)&lt;=0,MIN(G23:H23),SUMPRODUCT(C23:D23,G23:H23)),ABS(M23),IF(SUMPRODUCT(C23:D23,G23:H23)&lt;=0,MIN(G23:H23),SUMPRODUCT(C23:D23,G23:H23))),0)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="Q23">
@@ -1751,7 +1751,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F2F16FA-DA35-448D-B775-BE1ACD9ABBD8}">
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1822,7 +1824,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -1918,7 +1920,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -1940,7 +1942,7 @@
       </c>
       <c r="I9" s="2">
         <f>B5</f>
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="J9" s="2">
         <f>B6</f>
@@ -1948,14 +1950,14 @@
       </c>
       <c r="K9">
         <f>J9-I9</f>
-        <v>-31</v>
+        <v>31</v>
       </c>
       <c r="L9" s="7">
-        <f>IF(K9&lt;=0, 0, IF(K9&lt;=SUMPRODUCT(C9:D9,E9:F9),K9,SUMPRODUCT(C9:D9,E9:F9)))</f>
-        <v>0</v>
+        <f t="shared" ref="L9:L23" si="0">IF(K9&lt;=0, 0, IF(K9&lt;=SUMPRODUCT(C9:D9,E9:F9),K9,SUMPRODUCT(C9:D9,E9:F9)))</f>
+        <v>31</v>
       </c>
       <c r="M9">
-        <f>-IF(K9&lt;=0,0,-L9+K9)</f>
+        <f t="shared" ref="M9:M23" si="1">-IF(K9&lt;=0,0,-L9+K9)</f>
         <v>0</v>
       </c>
       <c r="N9">
@@ -1963,8 +1965,8 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <f>IF(K9&lt;=0,0,IF((((C9*N9)+(D9*N9))/N9),SUM(N9+L9),0))</f>
-        <v>0</v>
+        <f>IF(N9=0,L9,IF((((C9*N9)+(D9*N9))/N9),IF(COUNTIF(C10:D10, 1)=0, SUM(N9+L9),L9),0))</f>
+        <v>31</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="3"/>
@@ -1981,14 +1983,14 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <f t="shared" ref="E10:F23" si="0">$B$1</f>
+        <f t="shared" ref="E10:F23" si="2">$B$1</f>
         <v>118</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="G10">
@@ -1999,18 +2001,19 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>31</v>
+        <f>IF((I9-J9)&gt;=0,(I9-J9),0)</f>
+        <v>0</v>
       </c>
       <c r="J10">
         <v>31</v>
       </c>
       <c r="K10">
         <f>J10-I10</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="L10" s="7">
         <f>IF(K10&lt;=0, 0, IF(K10&lt;=SUMPRODUCT(C10:D10,E10:F10),K10,SUMPRODUCT(C10:D10,E10:F10)))</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="M10">
         <f>-IF(K10&lt;=0,0,-L10+K10)</f>
@@ -2021,8 +2024,8 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <f>IF(N10=0,0,IF(K10&lt;=0,0,IF((((C10*N10)+(D10*N10))/N10),SUM(N10+L10),0)))</f>
-        <v>0</v>
+        <f>IF(N10=0,L10,IF((((C10*N10)+(D10*N10))/N10),IF(COUNTIF(C11:D11, 1)=0, SUM(N10+L10),L10),0))</f>
+        <v>31</v>
       </c>
       <c r="Q10" s="5"/>
       <c r="T10" s="5"/>
@@ -2041,11 +2044,11 @@
         <v>0</v>
       </c>
       <c r="E11" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="F11" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="G11" s="7">
@@ -2055,35 +2058,32 @@
       <c r="H11" s="7">
         <v>1</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11">
+        <f>IF((I10-J10)&gt;=0,(I10-J10),0)</f>
         <v>0</v>
       </c>
       <c r="J11" s="7">
         <v>31</v>
       </c>
       <c r="K11">
-        <f>J11-I11</f>
+        <f t="shared" ref="K11:K23" si="3">J11-I11</f>
         <v>31</v>
       </c>
       <c r="L11" s="7">
-        <f>IF(K11&lt;=0, 0, IF(K11&lt;=SUMPRODUCT(C11:D11,E11:F11),K11,SUMPRODUCT(C11:D11,E11:F11)))</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="M11">
-        <f>-IF(K11&lt;=0,0,-L11+K11)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N11">
         <f>SUM(M11)</f>
         <v>0</v>
       </c>
-      <c r="O11">
-        <f>IF(N11=0,0,IF(K11&lt;=0,0,IF((((C11*N11)+(D11*N11))/N11),SUM(N11+L11),0)))</f>
-        <v>0</v>
-      </c>
       <c r="P11" s="7">
         <f>-L11+P14</f>
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="Q11" s="8"/>
       <c r="T11" s="5"/>
@@ -2125,15 +2125,15 @@
         <v>60</v>
       </c>
       <c r="K12">
-        <f>J12-I12</f>
+        <f t="shared" si="3"/>
         <v>-10</v>
       </c>
       <c r="L12" s="7">
-        <f>IF(K12&lt;=0, 0, IF(K12&lt;=SUMPRODUCT(C12:D12,E12:F12),K12,SUMPRODUCT(C12:D12,E12:F12)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M12">
-        <f>-IF(K12&lt;=0,0,-L12+K12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N12">
@@ -2141,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <f>IF(K12&lt;=0,0,IF((((C12*N12)+(D12*N12))/N12),SUM(N12+L12),0))</f>
+        <f>IF(N12=0,L12,IF((((C12*N12)+(D12*N12))/N12),IF(COUNTIF(C13:D13, 1)=0, SUM(N12+L12),L12),0))</f>
         <v>0</v>
       </c>
       <c r="P12" s="2"/>
@@ -2162,11 +2162,11 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="G13">
@@ -2177,6 +2177,7 @@
         <v>0</v>
       </c>
       <c r="I13">
+        <f>IF((I12-J12)&gt;=0,(I12-J12),0)</f>
         <v>10</v>
       </c>
       <c r="J13">
@@ -2187,11 +2188,11 @@
         <v>50</v>
       </c>
       <c r="L13" s="7">
-        <f>IF(K13&lt;=0, 0, IF(K13&lt;=SUMPRODUCT(C13:D13,E13:F13),K13,SUMPRODUCT(C13:D13,E13:F13)))</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="M13">
-        <f>-IF(K13&lt;=0,0,-L13+K13)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N13">
@@ -2199,8 +2200,8 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <f>IF(N13=0,0,IF(K13&lt;=0,0,IF((((C13*N13)+(D13*N13))/N13),SUM(N13+L13),0)))</f>
-        <v>0</v>
+        <f>IF(N13=0,L13,IF((((C13*N13)+(D13*N13))/N13),IF(COUNTIF(C14:D14, 1)=0, SUM(N13+L13),L13),0))</f>
+        <v>50</v>
       </c>
       <c r="Q13" s="5"/>
       <c r="T13" s="5"/>
@@ -2219,11 +2220,11 @@
         <v>0</v>
       </c>
       <c r="E14" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="F14" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="G14" s="7">
@@ -2233,35 +2234,32 @@
       <c r="H14" s="7">
         <v>1</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14">
+        <f>IF((I13-J13)&gt;=0,(I13-J13),0)</f>
         <v>0</v>
       </c>
       <c r="J14" s="7">
         <v>60</v>
       </c>
       <c r="K14">
-        <f>J14-I14</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="L14" s="7">
-        <f>IF(K14&lt;=0, 0, IF(K14&lt;=SUMPRODUCT(C14:D14,E14:F14),K14,SUMPRODUCT(C14:D14,E14:F14)))</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="M14">
-        <f>-IF(K14&lt;=0,0,-L14+K14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N14">
         <f>SUM(M14)</f>
         <v>0</v>
       </c>
-      <c r="O14">
-        <f>IF(N14=0,0,IF(K14&lt;=0,0,IF((((C14*N14)+(D14*N14))/N14),SUM(N14+L14),0)))</f>
-        <v>0</v>
-      </c>
       <c r="P14" s="7">
         <f>P23-L14</f>
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="Q14" s="8"/>
       <c r="T14" s="5"/>
@@ -2303,15 +2301,15 @@
         <v>17</v>
       </c>
       <c r="K15">
-        <f>J15-I15</f>
+        <f t="shared" si="3"/>
         <v>-17</v>
       </c>
       <c r="L15" s="7">
-        <f>IF(K15&lt;=0, 0, IF(K15&lt;=SUMPRODUCT(C15:D15,E15:F15),K15,SUMPRODUCT(C15:D15,E15:F15)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M15">
-        <f>-IF(K15&lt;=0,0,-L15+K15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N15">
@@ -2319,7 +2317,7 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <f>IF(N15=0,0,IF(K15&lt;=0,0,IF((((C15*N15)+(D15*N15))/N15),SUM(N15+L15),0)))</f>
+        <f t="shared" ref="O15:O16" si="4">IF(N15=0,L15,IF((((C15*N15)+(D15*N15))/N15),IF(COUNTIF(C16:D16, 1)=0, SUM(N15+L15),L15),0))</f>
         <v>0</v>
       </c>
       <c r="P15" s="2"/>
@@ -2340,11 +2338,11 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="G16">
@@ -2355,21 +2353,22 @@
         <v>0</v>
       </c>
       <c r="I16">
+        <f>IF((I15-J15)&gt;=0,(I15-J15),0)</f>
         <v>17</v>
       </c>
       <c r="J16">
         <v>17</v>
       </c>
       <c r="K16">
-        <f>J16-I16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L16" s="7">
-        <f>IF(K16&lt;=0, 0, IF(K16&lt;=SUMPRODUCT(C16:D16,E16:F16),K16,SUMPRODUCT(C16:D16,E16:F16)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M16">
-        <f>-IF(K16&lt;=0,0,-L16+K16)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N16">
@@ -2377,7 +2376,7 @@
         <v>0</v>
       </c>
       <c r="O16">
-        <f>IF(N16=0,0,IF(K16&lt;=0,0,IF((((C16*N16)+(D16*N16))/N16),SUM(N16+L16),0)))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q16" s="5"/>
@@ -2397,11 +2396,11 @@
         <v>1</v>
       </c>
       <c r="E17" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="F17" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="G17" s="7">
@@ -2411,30 +2410,27 @@
       <c r="H17" s="7">
         <v>0</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17">
+        <f>IF((I16-J16)&gt;=0,(I16-J16),0)</f>
         <v>0</v>
       </c>
       <c r="J17" s="7">
         <v>17</v>
       </c>
       <c r="K17">
-        <f>J17-I17</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="L17" s="7">
-        <f>IF(K17&lt;=0, 0, IF(K17&lt;=SUMPRODUCT(C17:D17,E17:F17),K17,SUMPRODUCT(C17:D17,E17:F17)))</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="M17">
-        <f>-IF(K17&lt;=0,0,-L17+K17)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N17">
         <f>SUM(M17)</f>
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <f>IF(N17=0,0,IF(K17&lt;=0,0,IF((((C17*N17)+(D17*N17))/N17),SUM(N17+L17),0)))</f>
         <v>0</v>
       </c>
       <c r="P17" s="7"/>
@@ -2458,11 +2454,11 @@
         <v>0</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="G18" s="2">
@@ -2481,15 +2477,15 @@
         <v>38</v>
       </c>
       <c r="K18">
-        <f>J18-I18</f>
+        <f t="shared" si="3"/>
         <v>-38</v>
       </c>
       <c r="L18" s="7">
-        <f>IF(K18&lt;=0, 0, IF(K18&lt;=SUMPRODUCT(C18:D18,E18:F18),K18,SUMPRODUCT(C18:D18,E18:F18)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M18">
-        <f>-IF(K18&lt;=0,0,-L18+K18)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N18">
@@ -2497,7 +2493,7 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <f>IF(N18=0,0,IF(K18&lt;=0,0,IF((((C18*N18)+(D18*N18))/N18),SUM(N18+L18),0)))</f>
+        <f t="shared" ref="O18:O19" si="5">IF(N18=0,L18,IF((((C18*N18)+(D18*N18))/N18),IF(COUNTIF(C19:D19, 1)=0, SUM(N18+L18),L18),0))</f>
         <v>0</v>
       </c>
       <c r="P18" s="2"/>
@@ -2518,11 +2514,11 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="G19">
@@ -2533,6 +2529,7 @@
         <v>0</v>
       </c>
       <c r="I19">
+        <f>IF((I18-J18)&gt;=0,(I18-J18),0)</f>
         <v>38</v>
       </c>
       <c r="J19">
@@ -2547,7 +2544,7 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <f>-IF(K19&lt;=0,0,-L19+K19)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N19">
@@ -2555,7 +2552,7 @@
         <v>0</v>
       </c>
       <c r="O19">
-        <f>IF(N19=0,0,IF(K19&lt;=0,0,IF((((C19*N19)+(D19*N19))/N19),SUM(N19+L19),0)))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q19" s="5"/>
@@ -2575,11 +2572,11 @@
         <v>1</v>
       </c>
       <c r="E20" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="F20" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="G20" s="7">
@@ -2589,30 +2586,27 @@
       <c r="H20" s="7">
         <v>0</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20">
+        <f>IF((I19-J19)&gt;=0,(I19-J19),0)</f>
         <v>0</v>
       </c>
       <c r="J20" s="7">
         <v>38</v>
       </c>
       <c r="K20">
-        <f>J20-I20</f>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="L20" s="7">
-        <f>IF(K20&lt;=0, 0, IF(K20&lt;=SUMPRODUCT(C20:D20,E20:F20),K20,SUMPRODUCT(C20:D20,E20:F20)))</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="M20">
-        <f>-IF(K20&lt;=0,0,-L20+K20)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N20">
         <f>SUM(M20)</f>
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <f>IF(N20=0,0,IF(K20&lt;=0,0,IF((((C20*N20)+(D20*N20))/N20),SUM(N20+L20),0)))</f>
         <v>0</v>
       </c>
       <c r="P20" s="7"/>
@@ -2635,11 +2629,11 @@
         <v>0</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="G21" s="2">
@@ -2662,11 +2656,11 @@
         <v>2</v>
       </c>
       <c r="L21" s="7">
-        <f>IF(K21&lt;=0, 0, IF(K21&lt;=SUMPRODUCT(C21:D21,E21:F21),K21,SUMPRODUCT(C21:D21,E21:F21)))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="M21">
-        <f>-IF(K21&lt;=0,0,-L21+K21)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N21">
@@ -2674,10 +2668,14 @@
         <v>12</v>
       </c>
       <c r="O21">
-        <f>IF(N21=0,0,IF(K21&lt;=0,0,IF((((C21*N21)+(D21*N21))/N21),SUM(N21+L21),0)))</f>
-        <v>14</v>
+        <f>IF(N21=0,L21,IF((((C21*N21)+(D21*N21))/N21),IF(COUNTIF(C22:D22, 1)=0, SUM(N21+L21),L21),0))</f>
+        <v>2</v>
       </c>
       <c r="Q21" s="3"/>
+      <c r="R21">
+        <f>IF((((C21*N21)+(D21*N21))/N21),IF(COUNTIF(C22:D22, 1)=0, SUM(N21+L21),0),0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
@@ -2690,14 +2688,14 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="G22">
@@ -2708,6 +2706,7 @@
         <v>0</v>
       </c>
       <c r="I22">
+        <f>IF((I21-J21)&gt;=0,(I21-J21),0)</f>
         <v>0</v>
       </c>
       <c r="J22">
@@ -2718,20 +2717,20 @@
         <v>12</v>
       </c>
       <c r="L22" s="7">
-        <f>IF(K22&lt;=0, 0, IF(K22&lt;=SUMPRODUCT(C22:D22,E22:F22),K22,SUMPRODUCT(C22:D22,E22:F22)))</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="M22">
-        <f>-IF(K22&lt;=0,0,-L22+K22)</f>
-        <v>-12</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="N22">
         <f>ABS(SUM(M22:M23))</f>
         <v>12</v>
       </c>
       <c r="O22">
-        <f>IF(N22=0,0,IF(K22&lt;=0,0,IF((((C22*N22)+(D22*N22))/N22),SUM(N22+L22),0)))</f>
-        <v>0</v>
+        <f t="shared" ref="O22" si="6">IF(N22=0,L22,IF((((C22*N22)+(D22*N22))/N22),IF(COUNTIF(C23:D23, 1)=0, SUM(N22+L22),L22),0))</f>
+        <v>24</v>
       </c>
       <c r="Q22" s="5"/>
     </row>
@@ -2743,17 +2742,17 @@
         <v>3</v>
       </c>
       <c r="C23" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="7">
         <v>0</v>
       </c>
       <c r="E23" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="F23" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="G23" s="7">
@@ -2763,35 +2762,32 @@
       <c r="H23" s="7">
         <v>1</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23">
+        <f>IF((I22-J22)&gt;=0,(I22-J22),0)</f>
         <v>0</v>
       </c>
       <c r="J23" s="7">
         <v>12</v>
       </c>
       <c r="K23">
-        <f>J23-I23</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="L23" s="7">
-        <f>IF(K23&lt;=0, 0, IF(K23&lt;=SUMPRODUCT(C23:D23,E23:F23),K23,SUMPRODUCT(C23:D23,E23:F23)))</f>
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="M23">
-        <f>-IF(K23&lt;=0,0,-L23+K23)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>-12</v>
       </c>
       <c r="N23">
         <f>SUM(M23)</f>
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <f>IF(N23=0,0,IF(K23&lt;=0,0,IF((((C23*N23)+(D23*N23))/N23),SUM(N23+L23),0)))</f>
-        <v>0</v>
+        <v>-12</v>
       </c>
       <c r="P23" s="7">
         <f>E23-L23</f>
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="Q23" s="8"/>
     </row>

</xml_diff>

<commit_message>
Excel Sheet - Added logic for final time period
</commit_message>
<xml_diff>
--- a/src/dynamiclot/excel/Algo_Test.xlsx
+++ b/src/dynamiclot/excel/Algo_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dynamicLot\dynamicLot\src\dynamiclot\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1663D2D5-AF3D-4644-80E5-172D86EB0C9A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08ACF171-3E18-4BEA-B5BC-B4FAE3A907F9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{02BB62FB-2EF9-455F-95E9-05B9DFC2DF15}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Down" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Down!$A$8:$S$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Down!$A$8:$N$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Top!$A$8:$O$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="30">
   <si>
     <t>.</t>
   </si>
@@ -126,12 +126,6 @@
   </si>
   <si>
     <t>Total for the TP</t>
-  </si>
-  <si>
-    <t>Vehicle1 Net Veh Cap</t>
-  </si>
-  <si>
-    <t>Vehicle2 Net Veh Cap</t>
   </si>
 </sst>
 </file>
@@ -253,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -264,6 +258,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1A9ADD-C05D-4DA2-985E-8370FA174CA3}">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1749,24 +1770,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F2F16FA-DA35-448D-B775-BE1ACD9ABBD8}">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="0" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="0" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1774,7 +1793,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1782,7 +1801,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -1799,7 +1818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1819,12 +1838,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -1839,7 +1858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1859,940 +1878,867 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H8" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="H8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J8" t="s">
+      <c r="I8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K8" t="s">
+      <c r="J8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="L8" t="s">
+      <c r="K8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="M8" t="s">
+      <c r="L8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="N8" t="s">
+      <c r="M8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="O8" t="s">
+      <c r="N8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="P8" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="B9" s="11">
+        <v>1</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="11">
         <f>$B$1</f>
         <v>118</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="11">
         <f>$B$1</f>
         <v>118</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="11">
         <f>$B$4</f>
         <v>93</v>
       </c>
-      <c r="H9" s="2">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2">
+      <c r="H9" s="11">
         <f>B5</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
+        <v>60</v>
+      </c>
+      <c r="I9" s="11">
         <f>B6</f>
         <v>31</v>
       </c>
-      <c r="K9">
-        <f>J9-I9</f>
-        <v>31</v>
-      </c>
-      <c r="L9" s="7">
-        <f t="shared" ref="L9:L23" si="0">IF(K9&lt;=0, 0, IF(K9&lt;=SUMPRODUCT(C9:D9,E9:F9),K9,SUMPRODUCT(C9:D9,E9:F9)))</f>
-        <v>31</v>
-      </c>
-      <c r="M9">
-        <f t="shared" ref="M9:M23" si="1">-IF(K9&lt;=0,0,-L9+K9)</f>
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <f>ABS(SUM(M9:M11))</f>
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <f>IF(N9=0,L9,IF((((C9*N9)+(D9*N9))/N9),IF(COUNTIF(C10:D10, 1)=0, SUM(N9+L9),L9),0))</f>
-        <v>31</v>
-      </c>
-      <c r="P9" s="2"/>
+      <c r="J9" s="11">
+        <f>I9-H9</f>
+        <v>-29</v>
+      </c>
+      <c r="K9" s="11">
+        <f>IF(J9&lt;=0, 0, IF(J9&lt;=SUMPRODUCT(C9:D9,E9:F9),J9,SUMPRODUCT(C9:D9,E9:F9)))</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="11">
+        <f t="shared" ref="L9:L23" si="0">-IF(J9&lt;=0,0,-K9+J9)</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="11">
+        <f>ABS(SUM(L9:L11))</f>
+        <v>2</v>
+      </c>
+      <c r="N9" s="12">
+        <f>IF(M9=0,K9,IF((((C9*M9)+(D9*M9))/M9),IF(COUNTIF(C10:D10, 1)=0, SUM(M9+K9),K9),0))</f>
+        <v>0</v>
+      </c>
       <c r="Q9" s="3"/>
-      <c r="T9" s="3"/>
-    </row>
-    <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="14">
         <v>2</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <f t="shared" ref="E10:F23" si="2">$B$1</f>
-        <v>118</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="G10">
+      <c r="C10" s="14">
+        <v>0</v>
+      </c>
+      <c r="D10" s="14">
+        <v>0</v>
+      </c>
+      <c r="E10" s="14">
+        <f t="shared" ref="E10:F23" si="1">$B$1</f>
+        <v>118</v>
+      </c>
+      <c r="F10" s="14">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="G10" s="14">
         <f>$B$4</f>
         <v>93</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <f>IF((I9-J9)&gt;=0,(I9-J9),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J10">
+      <c r="H10" s="14">
+        <f>IF((H9-I9)&gt;=0,(H9-I9),0)</f>
+        <v>29</v>
+      </c>
+      <c r="I10" s="14">
         <v>31</v>
       </c>
-      <c r="K10">
-        <f>J10-I10</f>
-        <v>31</v>
-      </c>
-      <c r="L10" s="7">
-        <f>IF(K10&lt;=0, 0, IF(K10&lt;=SUMPRODUCT(C10:D10,E10:F10),K10,SUMPRODUCT(C10:D10,E10:F10)))</f>
-        <v>31</v>
-      </c>
-      <c r="M10">
-        <f>-IF(K10&lt;=0,0,-L10+K10)</f>
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <f>ABS(SUM(M10:M11))</f>
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <f>IF(N10=0,L10,IF((((C10*N10)+(D10*N10))/N10),IF(COUNTIF(C11:D11, 1)=0, SUM(N10+L10),L10),0))</f>
-        <v>31</v>
+      <c r="J10" s="14">
+        <f>I10-H10</f>
+        <v>2</v>
+      </c>
+      <c r="K10" s="14">
+        <f>IF(J10&lt;=0, 0, IF(J10&lt;=SUMPRODUCT(C10:D10,E10:F10),J10,SUMPRODUCT(C10:D10,E10:F10)))</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="14">
+        <f>-IF(J10&lt;=0,0,-K10+J10)</f>
+        <v>-2</v>
+      </c>
+      <c r="M10" s="14">
+        <f>ABS(SUM(L10:L11))</f>
+        <v>2</v>
+      </c>
+      <c r="N10" s="15">
+        <f>IF(M10=0,K10,IF((((C10*M10)+(D10*M10))/M10),IF(COUNTIF(C11:D11, 1)=0, SUM(M10+K10),K10),0))</f>
+        <v>0</v>
       </c>
       <c r="Q10" s="5"/>
-      <c r="T10" s="5"/>
-    </row>
-    <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+    </row>
+    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="17">
         <v>3</v>
       </c>
-      <c r="C11" s="7">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0</v>
-      </c>
-      <c r="E11" s="7">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="F11" s="7">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="G11" s="7">
+      <c r="C11" s="17">
+        <v>0</v>
+      </c>
+      <c r="D11" s="17">
+        <v>1</v>
+      </c>
+      <c r="E11" s="17">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="F11" s="17">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="G11" s="17">
         <f>$B$4</f>
         <v>93</v>
       </c>
-      <c r="H11" s="7">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <f>IF((I10-J10)&gt;=0,(I10-J10),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="7">
+      <c r="H11" s="17">
+        <f>IF((H10-I10)&gt;=0,(H10-I10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="17">
         <v>31</v>
       </c>
-      <c r="K11">
-        <f t="shared" ref="K11:K23" si="3">J11-I11</f>
+      <c r="J11" s="17">
+        <f t="shared" ref="J11:J23" si="2">I11-H11</f>
         <v>31</v>
       </c>
-      <c r="L11" s="7">
+      <c r="K11" s="17">
+        <f>IF(J11&lt;=0, 0, IF(J11&lt;=SUMPRODUCT(C11:D11,E11:F11),J11,SUMPRODUCT(C11:D11,E11:F11)))</f>
+        <v>31</v>
+      </c>
+      <c r="L11" s="17">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="17">
+        <f>SUM(L11)</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="18">
+        <f>IF(K11&gt;0,K11,0)</f>
         <v>31</v>
       </c>
-      <c r="M11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <f>SUM(M11)</f>
-        <v>0</v>
-      </c>
-      <c r="P11" s="7">
-        <f>-L11+P14</f>
-        <v>27</v>
-      </c>
-      <c r="Q11" s="8"/>
-      <c r="T11" s="5"/>
-    </row>
-    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="Q11" s="5"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="B12" s="11">
+        <v>1</v>
+      </c>
+      <c r="C12" s="11">
+        <v>1</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0</v>
+      </c>
+      <c r="E12" s="11">
         <f>$B$1</f>
         <v>118</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="11">
         <f>$B$1</f>
         <v>118</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="11">
         <f>$C$4</f>
         <v>180</v>
       </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
-      <c r="I12" s="2">
+      <c r="H12" s="11">
         <f>C5</f>
         <v>70</v>
       </c>
-      <c r="J12" s="2">
+      <c r="I12" s="11">
         <f>C6</f>
         <v>60</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="3"/>
+      <c r="J12" s="11">
+        <f t="shared" si="2"/>
         <v>-10</v>
       </c>
-      <c r="L12" s="7">
+      <c r="K12" s="11">
+        <f>IF(J12&lt;=0, 0, IF(J12&lt;=SUMPRODUCT(C12:D12,E12:F12),J12,SUMPRODUCT(C12:D12,E12:F12)))</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="11">
+        <f>ABS(SUM(L12:L14))</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="12">
+        <f>IF(M12=0,K12,IF((((C12*M12)+(D12*M12))/M12),IF(COUNTIF(C13:D13, 1)=0, SUM(M12+K12),K12),0))</f>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="5"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="14">
+        <v>2</v>
+      </c>
+      <c r="C13" s="14">
+        <v>0</v>
+      </c>
+      <c r="D13" s="14">
+        <v>1</v>
+      </c>
+      <c r="E13" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <f>ABS(SUM(M12:M14))</f>
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <f>IF(N12=0,L12,IF((((C12*N12)+(D12*N12))/N12),IF(COUNTIF(C13:D13, 1)=0, SUM(N12+L12),L12),0))</f>
-        <v>0</v>
-      </c>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="3"/>
-      <c r="T12" s="5"/>
-    </row>
-    <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="G13">
+        <v>118</v>
+      </c>
+      <c r="F13" s="14">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="G13" s="14">
         <f>$C$4</f>
         <v>180</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <f>IF((I12-J12)&gt;=0,(I12-J12),0)</f>
+      <c r="H13" s="14">
+        <f>IF((H12-I12)&gt;=0,(H12-I12),0)</f>
         <v>10</v>
       </c>
-      <c r="J13">
+      <c r="I13" s="14">
         <v>60</v>
       </c>
-      <c r="K13">
-        <f>J13-I13</f>
+      <c r="J13" s="14">
+        <f>I13-H13</f>
         <v>50</v>
       </c>
-      <c r="L13" s="7">
+      <c r="K13" s="14">
+        <f>IF(J13&lt;=0, 0, IF(J13&lt;=SUMPRODUCT(C13:D13,E13:F13),J13,SUMPRODUCT(C13:D13,E13:F13)))</f>
+        <v>50</v>
+      </c>
+      <c r="L13" s="14">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="14">
+        <f>ABS(SUM(L13:L14))</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="15">
+        <f>IF(M13=0,K13,IF((((C13*M13)+(D13*M13))/M13),IF(COUNTIF(C14:D14, 1)=0, SUM(M13+K13),K13),0))</f>
         <v>50</v>
       </c>
-      <c r="M13">
+      <c r="Q13" s="5"/>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="17">
+        <v>3</v>
+      </c>
+      <c r="C14" s="17">
+        <v>1</v>
+      </c>
+      <c r="D14" s="17">
+        <v>0</v>
+      </c>
+      <c r="E14" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <f>ABS(SUM(M13:M14))</f>
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <f>IF(N13=0,L13,IF((((C13*N13)+(D13*N13))/N13),IF(COUNTIF(C14:D14, 1)=0, SUM(N13+L13),L13),0))</f>
-        <v>50</v>
-      </c>
-      <c r="Q13" s="5"/>
-      <c r="T13" s="5"/>
-    </row>
-    <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="7">
-        <v>3</v>
-      </c>
-      <c r="C14" s="7">
-        <v>1</v>
-      </c>
-      <c r="D14" s="7">
-        <v>0</v>
-      </c>
-      <c r="E14" s="7">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="F14" s="7">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="G14" s="7">
+        <v>118</v>
+      </c>
+      <c r="F14" s="17">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="G14" s="17">
         <f>$C$4</f>
         <v>180</v>
       </c>
-      <c r="H14" s="7">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <f>IF((I13-J13)&gt;=0,(I13-J13),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J14" s="7">
+      <c r="H14" s="17">
+        <f>IF((H13-I13)&gt;=0,(H13-I13),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="17">
         <v>60</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="3"/>
+      <c r="J14" s="17">
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="L14" s="7">
+      <c r="K14" s="17">
+        <f>IF(J14&lt;=0, 0, IF(J14&lt;=SUMPRODUCT(C14:D14,E14:F14),J14,SUMPRODUCT(C14:D14,E14:F14)))</f>
+        <v>60</v>
+      </c>
+      <c r="L14" s="17">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="17">
+        <f>SUM(L14)</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="18">
+        <f>IF(K14&gt;0,K14,0)</f>
         <v>60</v>
       </c>
-      <c r="M14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <f>SUM(M14)</f>
-        <v>0</v>
-      </c>
-      <c r="P14" s="7">
-        <f>P23-L14</f>
-        <v>58</v>
-      </c>
-      <c r="Q14" s="8"/>
-      <c r="T14" s="5"/>
-    </row>
-    <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2">
+      <c r="B15" s="11">
+        <v>1</v>
+      </c>
+      <c r="C15" s="11">
+        <v>0</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0</v>
+      </c>
+      <c r="E15" s="11">
         <f>$B$1</f>
         <v>118</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="11">
         <f>$B$1</f>
         <v>118</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="11">
         <f>$D$4</f>
         <v>51</v>
       </c>
-      <c r="H15" s="2">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2">
+      <c r="H15" s="11">
         <f>D5</f>
         <v>34</v>
       </c>
-      <c r="J15" s="2">
+      <c r="I15" s="11">
         <f>D6</f>
         <v>17</v>
       </c>
-      <c r="K15">
-        <f t="shared" si="3"/>
+      <c r="J15" s="11">
+        <f t="shared" si="2"/>
         <v>-17</v>
       </c>
-      <c r="L15" s="7">
+      <c r="K15" s="11">
+        <f>IF(J15&lt;=0, 0, IF(J15&lt;=SUMPRODUCT(C15:D15,E15:F15),J15,SUMPRODUCT(C15:D15,E15:F15)))</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="11">
+        <f>ABS(SUM(L15:L17))</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="12">
+        <f>IF(M15=0,K15,IF((((C15*M15)+(D15*M15))/M15),IF(COUNTIF(C16:D16, 1)=0, SUM(M15+K15),K15),0))</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="5"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="14">
+        <v>2</v>
+      </c>
+      <c r="C16" s="14">
+        <v>0</v>
+      </c>
+      <c r="D16" s="14">
+        <v>0</v>
+      </c>
+      <c r="E16" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <f>ABS(SUM(M15:M17))</f>
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <f t="shared" ref="O15:O16" si="4">IF(N15=0,L15,IF((((C15*N15)+(D15*N15))/N15),IF(COUNTIF(C16:D16, 1)=0, SUM(N15+L15),L15),0))</f>
-        <v>0</v>
-      </c>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="3"/>
-      <c r="T15" s="5"/>
-    </row>
-    <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="G16">
+        <v>118</v>
+      </c>
+      <c r="F16" s="14">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="G16" s="14">
         <f>$D$4</f>
         <v>51</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <f>IF((I15-J15)&gt;=0,(I15-J15),0)</f>
+      <c r="H16" s="14">
+        <f>IF((H15-I15)&gt;=0,(H15-I15),0)</f>
         <v>17</v>
       </c>
-      <c r="J16">
+      <c r="I16" s="14">
         <v>17</v>
       </c>
-      <c r="K16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L16" s="7">
+      <c r="J16" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="14">
+        <f>IF(J16&lt;=0, 0, IF(J16&lt;=SUMPRODUCT(C16:D16,E16:F16),J16,SUMPRODUCT(C16:D16,E16:F16)))</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="14">
+        <f>ABS(SUM(L16:L17))</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="15">
+        <f>IF(M16=0,K16,IF((((C16*M16)+(D16*M16))/M16),IF(COUNTIF(C17:D17, 1)=0, SUM(M16+K16),K16),0))</f>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="5"/>
+    </row>
+    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="17">
+        <v>3</v>
+      </c>
+      <c r="C17" s="17">
+        <v>0</v>
+      </c>
+      <c r="D17" s="17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <f>ABS(SUM(M16:M17))</f>
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="5"/>
-      <c r="T16" s="5"/>
-    </row>
-    <row r="17" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="7">
-        <v>3</v>
-      </c>
-      <c r="C17" s="7">
-        <v>0</v>
-      </c>
-      <c r="D17" s="7">
-        <v>1</v>
-      </c>
-      <c r="E17" s="7">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="F17" s="7">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="G17" s="7">
+        <v>118</v>
+      </c>
+      <c r="F17" s="17">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="G17" s="17">
         <f>$D$4</f>
         <v>51</v>
       </c>
-      <c r="H17" s="7">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <f>IF((I16-J16)&gt;=0,(I16-J16),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J17" s="7">
+      <c r="H17" s="17">
+        <f>IF((H16-I16)&gt;=0,(H16-I16),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="17">
         <v>17</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="3"/>
+      <c r="J17" s="17">
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="L17" s="7">
+      <c r="K17" s="17">
+        <f>IF(J17&lt;=0, 0, IF(J17&lt;=SUMPRODUCT(C17:D17,E17:F17),J17,SUMPRODUCT(C17:D17,E17:F17)))</f>
+        <v>17</v>
+      </c>
+      <c r="L17" s="17">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="17">
+        <f>SUM(L17)</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="18">
+        <f>IF(K17&gt;0,K17,0)</f>
         <v>17</v>
       </c>
-      <c r="M17">
+      <c r="Q17" s="5"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="11">
+        <v>1</v>
+      </c>
+      <c r="C18" s="11">
+        <v>0</v>
+      </c>
+      <c r="D18" s="11">
+        <v>0</v>
+      </c>
+      <c r="E18" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <f>SUM(M17)</f>
-        <v>0</v>
-      </c>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="8">
-        <f>Q20-L17</f>
-        <v>63</v>
-      </c>
-      <c r="T17" s="5"/>
-    </row>
-    <row r="18" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="F18" s="2">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="G18" s="2">
+        <v>118</v>
+      </c>
+      <c r="F18" s="11">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="G18" s="11">
         <f>$E$4</f>
         <v>114</v>
       </c>
-      <c r="H18" s="2">
-        <v>0</v>
-      </c>
-      <c r="I18" s="2">
+      <c r="H18" s="11">
         <f>E5</f>
         <v>76</v>
       </c>
-      <c r="J18" s="2">
+      <c r="I18" s="11">
         <f>E6</f>
         <v>38</v>
       </c>
-      <c r="K18">
-        <f t="shared" si="3"/>
+      <c r="J18" s="11">
+        <f t="shared" si="2"/>
         <v>-38</v>
       </c>
-      <c r="L18" s="7">
+      <c r="K18" s="11">
+        <f>IF(J18&lt;=0, 0, IF(J18&lt;=SUMPRODUCT(C18:D18,E18:F18),J18,SUMPRODUCT(C18:D18,E18:F18)))</f>
+        <v>0</v>
+      </c>
+      <c r="L18" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="11">
+        <f>ABS(SUM(L18:L20))</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="12">
+        <f>IF(M18=0,K18,IF((((C18*M18)+(D18*M18))/M18),IF(COUNTIF(C19:D19, 1)=0, SUM(M18+K18),K18),0))</f>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="5"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="14">
+        <v>2</v>
+      </c>
+      <c r="C19" s="14">
+        <v>0</v>
+      </c>
+      <c r="D19" s="14">
+        <v>0</v>
+      </c>
+      <c r="E19" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <f>ABS(SUM(M18:M20))</f>
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <f t="shared" ref="O18:O19" si="5">IF(N18=0,L18,IF((((C18*N18)+(D18*N18))/N18),IF(COUNTIF(C19:D19, 1)=0, SUM(N18+L18),L18),0))</f>
-        <v>0</v>
-      </c>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="3"/>
-      <c r="T18" s="5"/>
-    </row>
-    <row r="19" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="G19">
+        <v>118</v>
+      </c>
+      <c r="F19" s="14">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="G19" s="14">
         <f>$E$4</f>
         <v>114</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <f>IF((I18-J18)&gt;=0,(I18-J18),0)</f>
+      <c r="H19" s="14">
+        <f>IF((H18-I18)&gt;=0,(H18-I18),0)</f>
         <v>38</v>
       </c>
-      <c r="J19">
+      <c r="I19" s="14">
         <v>38</v>
       </c>
-      <c r="K19">
-        <f>J19-I19</f>
-        <v>0</v>
-      </c>
-      <c r="L19" s="7">
-        <f>IF(K19&lt;=0, 0, IF(K19&lt;=SUMPRODUCT(C19:D19,E19:F19),K19,SUMPRODUCT(C19:D19,E19:F19)))</f>
-        <v>0</v>
-      </c>
-      <c r="M19">
+      <c r="J19" s="14">
+        <f>I19-H19</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="14">
+        <f>IF(J19&lt;=0, 0, IF(J19&lt;=SUMPRODUCT(C19:D19,E19:F19),J19,SUMPRODUCT(C19:D19,E19:F19)))</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="14">
+        <f>ABS(SUM(L19:L20))</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="15">
+        <f>IF(M19=0,K19,IF((((C19*M19)+(D19*M19))/M19),IF(COUNTIF(C20:D20, 1)=0, SUM(M19+K19),K19),0))</f>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="17">
+        <v>3</v>
+      </c>
+      <c r="C20" s="17">
+        <v>0</v>
+      </c>
+      <c r="D20" s="17">
+        <v>1</v>
+      </c>
+      <c r="E20" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <f>ABS(SUM(M19:M20))</f>
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="5"/>
-      <c r="T19" s="5"/>
-    </row>
-    <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="7">
-        <v>3</v>
-      </c>
-      <c r="C20" s="7">
-        <v>0</v>
-      </c>
-      <c r="D20" s="7">
-        <v>1</v>
-      </c>
-      <c r="E20" s="7">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="F20" s="7">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="G20" s="7">
+        <v>118</v>
+      </c>
+      <c r="F20" s="17">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="G20" s="17">
         <f>$E$4</f>
         <v>114</v>
       </c>
-      <c r="H20" s="7">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <f>IF((I19-J19)&gt;=0,(I19-J19),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J20" s="7">
+      <c r="H20" s="17">
+        <f>IF((H19-I19)&gt;=0,(H19-I19),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="17">
         <v>38</v>
       </c>
-      <c r="K20">
-        <f t="shared" si="3"/>
+      <c r="J20" s="17">
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="L20" s="7">
+      <c r="K20" s="17">
+        <f>IF(J20&lt;=0, 0, IF(J20&lt;=SUMPRODUCT(C20:D20,E20:F20),J20,SUMPRODUCT(C20:D20,E20:F20)))</f>
+        <v>38</v>
+      </c>
+      <c r="L20" s="17">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="17">
+        <f>SUM(L20)</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="18">
+        <f>IF(K20&gt;0,K20,0)</f>
         <v>38</v>
       </c>
-      <c r="M20">
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="11">
+        <v>1</v>
+      </c>
+      <c r="C21" s="11">
+        <v>1</v>
+      </c>
+      <c r="D21" s="11">
+        <v>0</v>
+      </c>
+      <c r="E21" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <f>SUM(M20)</f>
-        <v>0</v>
-      </c>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="8">
-        <f>F20-L20</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="2">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="F21" s="2">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="G21" s="2">
+        <v>118</v>
+      </c>
+      <c r="F21" s="11">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="G21" s="11">
         <f>$F$4</f>
         <v>24</v>
       </c>
-      <c r="H21" s="2">
-        <v>0</v>
-      </c>
-      <c r="I21" s="2">
+      <c r="H21" s="11">
         <f>F5</f>
         <v>10</v>
       </c>
-      <c r="J21" s="2">
+      <c r="I21" s="11">
         <f>F6</f>
         <v>12</v>
       </c>
-      <c r="K21">
-        <f>J21-I21</f>
+      <c r="J21" s="11">
+        <f>I21-H21</f>
         <v>2</v>
       </c>
-      <c r="L21" s="7">
+      <c r="K21" s="11">
+        <f>IF(J21&lt;=0, 0, IF(J21&lt;=SUMPRODUCT(C21:D21,E21:F21),J21,SUMPRODUCT(C21:D21,E21:F21)))</f>
+        <v>2</v>
+      </c>
+      <c r="L21" s="11">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="11">
+        <f>ABS(SUM(L21:L23))</f>
+        <v>12</v>
+      </c>
+      <c r="N21" s="12">
+        <f>IF(M21=0,K21,IF((((C21*M21)+(D21*M21))/M21),IF(COUNTIF(C22:D22, 1)=0, SUM(M21+K21),K21),0))</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="14">
         <v>2</v>
       </c>
-      <c r="M21">
+      <c r="C22" s="14">
+        <v>0</v>
+      </c>
+      <c r="D22" s="14">
+        <v>0</v>
+      </c>
+      <c r="E22" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <f>ABS(SUM(M21:M23))</f>
-        <v>12</v>
-      </c>
-      <c r="O21">
-        <f>IF(N21=0,L21,IF((((C21*N21)+(D21*N21))/N21),IF(COUNTIF(C22:D22, 1)=0, SUM(N21+L21),L21),0))</f>
-        <v>2</v>
-      </c>
-      <c r="Q21" s="3"/>
-      <c r="R21">
-        <f>IF((((C21*N21)+(D21*N21))/N21),IF(COUNTIF(C22:D22, 1)=0, SUM(N21+L21),0),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="G22">
+        <v>118</v>
+      </c>
+      <c r="F22" s="14">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="G22" s="14">
         <f>$F$4</f>
         <v>24</v>
       </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <f>IF((I21-J21)&gt;=0,(I21-J21),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J22">
+      <c r="H22" s="14">
+        <f>IF((H21-I21)&gt;=0,(H21-I21),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="14">
         <v>12</v>
       </c>
-      <c r="K22">
-        <f>J22-I22</f>
+      <c r="J22" s="14">
+        <f>I22-H22</f>
         <v>12</v>
       </c>
-      <c r="L22" s="7">
+      <c r="K22" s="14">
+        <f>IF(J22&lt;=0, 0, IF(J22&lt;=SUMPRODUCT(C22:D22,E22:F22),J22,SUMPRODUCT(C22:D22,E22:F22)))</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="14">
         <f t="shared" si="0"/>
+        <v>-12</v>
+      </c>
+      <c r="M22" s="14">
+        <f>ABS(SUM(L22:L23))</f>
         <v>12</v>
       </c>
-      <c r="M22">
+      <c r="N22" s="15">
+        <f>IF(M22=0,K22,IF((((C22*M22)+(D22*M22))/M22),IF(COUNTIF(C23:D23, 1)=0, SUM(M22+K22),K22),0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="17">
+        <v>3</v>
+      </c>
+      <c r="C23" s="17">
+        <v>1</v>
+      </c>
+      <c r="D23" s="17">
+        <v>0</v>
+      </c>
+      <c r="E23" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <f>ABS(SUM(M22:M23))</f>
-        <v>12</v>
-      </c>
-      <c r="O22">
-        <f t="shared" ref="O22" si="6">IF(N22=0,L22,IF((((C22*N22)+(D22*N22))/N22),IF(COUNTIF(C23:D23, 1)=0, SUM(N22+L22),L22),0))</f>
-        <v>24</v>
-      </c>
-      <c r="Q22" s="5"/>
-    </row>
-    <row r="23" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="7">
-        <v>3</v>
-      </c>
-      <c r="C23" s="7">
-        <v>0</v>
-      </c>
-      <c r="D23" s="7">
-        <v>0</v>
-      </c>
-      <c r="E23" s="7">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="F23" s="7">
-        <f t="shared" si="2"/>
-        <v>118</v>
-      </c>
-      <c r="G23" s="7">
+        <v>118</v>
+      </c>
+      <c r="F23" s="17">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="G23" s="17">
         <f>$F$4</f>
         <v>24</v>
       </c>
-      <c r="H23" s="7">
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <f>IF((I22-J22)&gt;=0,(I22-J22),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J23" s="7">
+      <c r="H23" s="17">
+        <f>IF((H22-I22)&gt;=0,(H22-I22),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="17">
         <v>12</v>
       </c>
-      <c r="K23">
-        <f t="shared" si="3"/>
+      <c r="J23" s="17">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="L23" s="7">
+      <c r="K23" s="17">
+        <f>IF(J23&lt;=0, 0, IF(J23&lt;=SUMPRODUCT(C23:D23,E23:F23),J23,SUMPRODUCT(C23:D23,E23:F23)))</f>
+        <v>12</v>
+      </c>
+      <c r="L23" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M23">
-        <f t="shared" si="1"/>
-        <v>-12</v>
-      </c>
-      <c r="N23">
-        <f>SUM(M23)</f>
-        <v>-12</v>
-      </c>
-      <c r="P23" s="7">
-        <f>E23-L23</f>
-        <v>118</v>
-      </c>
-      <c r="Q23" s="8"/>
+      <c r="M23" s="17">
+        <f>SUM(L23)</f>
+        <v>0</v>
+      </c>
+      <c r="N23" s="18">
+        <f>IF(K23&gt;0,K23,0)</f>
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A8:S23" xr:uid="{F0066AE3-89CB-4BA1-8D28-7547531DDD6D}"/>
+  <autoFilter ref="A8:N8" xr:uid="{D34B2026-AF3F-4C1A-90E4-69306730055A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="N9:N23" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>